<commit_message>
Requerimientos funcionales del 1 al 29
</commit_message>
<xml_diff>
--- a/django-tickets-app/media/solicitudes/plantilla_creacion_tablas.xlsx
+++ b/django-tickets-app/media/solicitudes/plantilla_creacion_tablas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\db_request_tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB476D3B-30A1-43F1-A110-31E5E3B3D15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0175E59D-A9CA-499B-9C23-54B650249C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-105" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Nombre de la columna</t>
   </si>
@@ -43,20 +43,56 @@
     <t>nombre tabla</t>
   </si>
   <si>
-    <t>coemtario tabla</t>
-  </si>
-  <si>
     <t>es foranea</t>
   </si>
   <si>
     <t>tabla referencia</t>
+  </si>
+  <si>
+    <t>tablaprueba</t>
+  </si>
+  <si>
+    <t>Esta tabla se crea para hacer una prueba</t>
+  </si>
+  <si>
+    <t>columna1</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>LLAVE PRIMARIA</t>
+  </si>
+  <si>
+    <t>columna2</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>otra columna</t>
+  </si>
+  <si>
+    <t>comentario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +102,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -108,12 +152,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H7"/>
+  <dimension ref="A2:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,8 +477,7 @@
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -440,18 +487,24 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -470,18 +523,62 @@
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B3:D4"/>
+    <mergeCell ref="A3:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>